<commit_message>
Loaded imada - dic data sets and enabled graphically determination of the time-offset. renamed files.
</commit_message>
<xml_diff>
--- a/examples/imada_ut/output/myexcel-withTimes.xlsx
+++ b/examples/imada_ut/output/myexcel-withTimes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_sandbox\hmu\hmu.materialslab.tools\examples\imada_ut\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_sandbox\research\hmu.materialslab.tools\examples\imada_ut\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9713CC2-A7EB-4960-8E2B-AED47645B260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30481D4A-EF8C-4778-80B4-C7AE38B456D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="7935" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -926,6 +926,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1274,19 +1275,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I146" sqref="I146:J154"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.36328125" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1305,14 +1307,14 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>294</v>
+      </c>
       <c r="I1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1334,14 +1336,14 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="2">
+      <c r="I2" s="2">
         <v>-9.8860740000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1363,14 +1365,14 @@
       <c r="G3">
         <v>2.2616582916681731E-4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
         <v>151</v>
       </c>
-      <c r="J3" s="2">
+      <c r="I3" s="2">
         <v>-1.0170940000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1392,14 +1394,14 @@
       <c r="G4">
         <v>4.7997199699056778E-4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="2">
+      <c r="I4" s="2">
         <v>2.2577229999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1421,14 +1423,14 @@
       <c r="G5">
         <v>4.0821737128361469E-4</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>153</v>
       </c>
-      <c r="J5" s="2">
+      <c r="I5" s="2">
         <v>2.3126929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1450,14 +1452,14 @@
       <c r="G6">
         <v>6.0332439772039365E-4</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>154</v>
       </c>
-      <c r="J6" s="2">
+      <c r="I6" s="2">
         <v>2.4126370000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1479,14 +1481,14 @@
       <c r="G7">
         <v>7.4718692637782877E-4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" t="s">
         <v>155</v>
       </c>
-      <c r="J7" s="2">
+      <c r="I7" s="2">
         <v>2.5046919999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1508,14 +1510,14 @@
       <c r="G8">
         <v>8.7151973213200516E-4</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" t="s">
         <v>156</v>
       </c>
-      <c r="J8" s="2">
+      <c r="I8" s="2">
         <v>2.6016360000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1537,14 +1539,14 @@
       <c r="G9">
         <v>9.1668731510869555E-4</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" t="s">
         <v>157</v>
       </c>
-      <c r="J9" s="2">
+      <c r="I9" s="2">
         <v>2.7141899999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1566,14 +1568,14 @@
       <c r="G10">
         <v>9.6650691293338287E-4</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" t="s">
         <v>158</v>
       </c>
-      <c r="J10" s="2">
+      <c r="I10" s="2">
         <v>2.8301270000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1595,14 +1597,14 @@
       <c r="G11">
         <v>1.028546275008682E-3</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" t="s">
         <v>159</v>
       </c>
-      <c r="J11" s="2">
+      <c r="I11" s="2">
         <v>2.9380670000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1624,14 +1626,14 @@
       <c r="G12">
         <v>9.4561857293639609E-4</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12" t="s">
         <v>160</v>
       </c>
-      <c r="J12" s="2">
+      <c r="I12" s="2">
         <v>3.037013</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1653,14 +1655,14 @@
       <c r="G13">
         <v>9.5810543469415784E-4</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" t="s">
         <v>161</v>
       </c>
-      <c r="J13" s="2">
+      <c r="I13" s="2">
         <v>3.1439530000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1682,14 +1684,14 @@
       <c r="G14">
         <v>1.1021920696216349E-3</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14" t="s">
         <v>162</v>
       </c>
-      <c r="J14" s="2">
+      <c r="I14" s="2">
         <v>3.1989299999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1711,14 +1713,14 @@
       <c r="G15">
         <v>1.046465058260069E-3</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15" t="s">
         <v>163</v>
       </c>
-      <c r="J15" s="2">
+      <c r="I15" s="2">
         <v>3.3068610000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1740,14 +1742,14 @@
       <c r="G16">
         <v>1.1823553741109401E-3</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H16" t="s">
         <v>164</v>
       </c>
-      <c r="J16" s="2">
+      <c r="I16" s="2">
         <v>3.402809</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1769,14 +1771,14 @@
       <c r="G17">
         <v>1.2174121640850159E-3</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H17" t="s">
         <v>165</v>
       </c>
-      <c r="J17" s="2">
+      <c r="I17" s="2">
         <v>3.5013239999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1798,14 +1800,14 @@
       <c r="G18">
         <v>1.055824304757609E-3</v>
       </c>
-      <c r="I18" t="s">
+      <c r="H18" t="s">
         <v>166</v>
       </c>
-      <c r="J18" s="2">
+      <c r="I18" s="2">
         <v>3.6152730000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1827,14 +1829,14 @@
       <c r="G19">
         <v>1.348501250184566E-3</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H19" t="s">
         <v>167</v>
       </c>
-      <c r="J19" s="2">
+      <c r="I19" s="2">
         <v>3.7072059999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1856,14 +1858,14 @@
       <c r="G20">
         <v>9.9607194828515901E-4</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H20" t="s">
         <v>168</v>
       </c>
-      <c r="J20" s="2">
+      <c r="I20" s="2">
         <v>3.8341370000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1885,14 +1887,14 @@
       <c r="G21">
         <v>1.084463038221447E-3</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H21" t="s">
         <v>169</v>
       </c>
-      <c r="J21" s="2">
+      <c r="I21" s="2">
         <v>3.9280840000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1914,14 +1916,14 @@
       <c r="G22">
         <v>1.1404877971580201E-3</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H22" t="s">
         <v>170</v>
       </c>
-      <c r="J22" s="2">
+      <c r="I22" s="2">
         <v>4.0160349999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1943,14 +1945,14 @@
       <c r="G23">
         <v>1.1122186244201511E-3</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H23" t="s">
         <v>171</v>
       </c>
-      <c r="J23" s="2">
+      <c r="I23" s="2">
         <v>4.1109859999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1972,14 +1974,14 @@
       <c r="G24">
         <v>1.231368427888401E-3</v>
       </c>
-      <c r="I24" t="s">
+      <c r="H24" t="s">
         <v>172</v>
       </c>
-      <c r="J24" s="2">
+      <c r="I24" s="2">
         <v>4.2099279999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2001,14 +2003,14 @@
       <c r="G25">
         <v>1.274822169217843E-3</v>
       </c>
-      <c r="I25" t="s">
+      <c r="H25" t="s">
         <v>173</v>
       </c>
-      <c r="J25" s="2">
+      <c r="I25" s="2">
         <v>4.3138699999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2030,14 +2032,14 @@
       <c r="G26">
         <v>1.442655535570266E-3</v>
       </c>
-      <c r="I26" t="s">
+      <c r="H26" t="s">
         <v>174</v>
       </c>
-      <c r="J26" s="2">
+      <c r="I26" s="2">
         <v>4.4138149999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2059,14 +2061,14 @@
       <c r="G27">
         <v>1.520950659674196E-3</v>
       </c>
-      <c r="I27" t="s">
+      <c r="H27" t="s">
         <v>175</v>
       </c>
-      <c r="J27" s="2">
+      <c r="I27" s="2">
         <v>4.5033450000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2088,14 +2090,14 @@
       <c r="G28">
         <v>1.491682385874748E-3</v>
       </c>
-      <c r="I28" t="s">
+      <c r="H28" t="s">
         <v>176</v>
       </c>
-      <c r="J28" s="2">
+      <c r="I28" s="2">
         <v>4.6294190000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2117,14 +2119,14 @@
       <c r="G29">
         <v>1.2866140935562369E-3</v>
       </c>
-      <c r="I29" t="s">
+      <c r="H29" t="s">
         <v>177</v>
       </c>
-      <c r="J29" s="2">
+      <c r="I29" s="2">
         <v>4.7238759999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2146,14 +2148,14 @@
       <c r="G30">
         <v>1.3448478452996191E-3</v>
       </c>
-      <c r="I30" t="s">
+      <c r="H30" t="s">
         <v>178</v>
       </c>
-      <c r="J30" s="2">
+      <c r="I30" s="2">
         <v>4.8058360000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2175,14 +2177,14 @@
       <c r="G31">
         <v>1.409396867424128E-3</v>
       </c>
-      <c r="I31" t="s">
+      <c r="H31" t="s">
         <v>179</v>
       </c>
-      <c r="J31" s="2">
+      <c r="I31" s="2">
         <v>4.8997789999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2204,14 +2206,14 @@
       <c r="G32">
         <v>1.4339817990805901E-3</v>
       </c>
-      <c r="I32" t="s">
+      <c r="H32" t="s">
         <v>180</v>
       </c>
-      <c r="J32" s="2">
+      <c r="I32" s="2">
         <v>4.999727</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2233,14 +2235,14 @@
       <c r="G33">
         <v>1.551335941741666E-3</v>
       </c>
-      <c r="I33" t="s">
+      <c r="H33" t="s">
         <v>181</v>
       </c>
-      <c r="J33" s="2">
+      <c r="I33" s="2">
         <v>5.1006689999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2262,14 +2264,14 @@
       <c r="G34">
         <v>1.6151542938856549E-3</v>
       </c>
-      <c r="I34" t="s">
+      <c r="H34" t="s">
         <v>182</v>
       </c>
-      <c r="J34" s="2">
+      <c r="I34" s="2">
         <v>5.200615</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2291,14 +2293,14 @@
       <c r="G35">
         <v>1.7410306829268171E-3</v>
       </c>
-      <c r="I35" t="s">
+      <c r="H35" t="s">
         <v>183</v>
       </c>
-      <c r="J35" s="2">
+      <c r="I35" s="2">
         <v>5.3035579999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2320,14 +2322,14 @@
       <c r="G36">
         <v>1.6768072891718609E-3</v>
       </c>
-      <c r="I36" t="s">
+      <c r="H36" t="s">
         <v>184</v>
       </c>
-      <c r="J36" s="2">
+      <c r="I36" s="2">
         <v>5.4035019999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2349,14 +2351,14 @@
       <c r="G37">
         <v>2.049375563029021E-3</v>
       </c>
-      <c r="I37" t="s">
+      <c r="H37" t="s">
         <v>185</v>
       </c>
-      <c r="J37" s="2">
+      <c r="I37" s="2">
         <v>5.5010110000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2378,14 +2380,14 @@
       <c r="G38">
         <v>2.0452696150272029E-3</v>
       </c>
-      <c r="I38" t="s">
+      <c r="H38" t="s">
         <v>186</v>
       </c>
-      <c r="J38" s="2">
+      <c r="I38" s="2">
         <v>5.6005520000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2407,14 +2409,14 @@
       <c r="G39">
         <v>1.968561878366199E-3</v>
       </c>
-      <c r="I39" t="s">
+      <c r="H39" t="s">
         <v>187</v>
       </c>
-      <c r="J39" s="2">
+      <c r="I39" s="2">
         <v>5.7005049999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2436,14 +2438,14 @@
       <c r="G40">
         <v>1.998093685163232E-3</v>
       </c>
-      <c r="I40" t="s">
+      <c r="H40" t="s">
         <v>188</v>
       </c>
-      <c r="J40" s="2">
+      <c r="I40" s="2">
         <v>5.8004490000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2465,14 +2467,14 @@
       <c r="G41">
         <v>1.935727914272777E-3</v>
       </c>
-      <c r="I41" t="s">
+      <c r="H41" t="s">
         <v>189</v>
       </c>
-      <c r="J41" s="2">
+      <c r="I41" s="2">
         <v>5.9010090000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2494,14 +2496,14 @@
       <c r="G42">
         <v>2.0545958122343828E-3</v>
       </c>
-      <c r="I42" t="s">
+      <c r="H42" t="s">
         <v>190</v>
       </c>
-      <c r="J42" s="2">
+      <c r="I42" s="2">
         <v>6.0019559999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2523,14 +2525,14 @@
       <c r="G43">
         <v>2.277713604271453E-3</v>
       </c>
-      <c r="I43" t="s">
+      <c r="H43" t="s">
         <v>191</v>
       </c>
-      <c r="J43" s="2">
+      <c r="I43" s="2">
         <v>6.1009019999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2552,14 +2554,14 @@
       <c r="G44">
         <v>2.2814845670358569E-3</v>
       </c>
-      <c r="I44" t="s">
+      <c r="H44" t="s">
         <v>192</v>
       </c>
-      <c r="J44" s="2">
+      <c r="I44" s="2">
         <v>6.2018440000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2581,14 +2583,14 @@
       <c r="G45">
         <v>2.4823075431315892E-3</v>
       </c>
-      <c r="I45" t="s">
+      <c r="H45" t="s">
         <v>193</v>
       </c>
-      <c r="J45" s="2">
+      <c r="I45" s="2">
         <v>6.3017859999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2610,14 +2612,14 @@
       <c r="G46">
         <v>2.6127224041367809E-3</v>
       </c>
-      <c r="I46" t="s">
+      <c r="H46" t="s">
         <v>194</v>
       </c>
-      <c r="J46" s="2">
+      <c r="I46" s="2">
         <v>6.3997320000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2639,14 +2641,14 @@
       <c r="G47">
         <v>2.7924735354853351E-3</v>
       </c>
-      <c r="I47" t="s">
+      <c r="H47" t="s">
         <v>195</v>
       </c>
-      <c r="J47" s="2">
+      <c r="I47" s="2">
         <v>6.5012699999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2668,14 +2670,14 @@
       <c r="G48">
         <v>2.7529126363685921E-3</v>
       </c>
-      <c r="I48" t="s">
+      <c r="H48" t="s">
         <v>196</v>
       </c>
-      <c r="J48" s="2">
+      <c r="I48" s="2">
         <v>6.6012170000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2697,14 +2699,14 @@
       <c r="G49">
         <v>2.5477906946928691E-3</v>
       </c>
-      <c r="I49" t="s">
+      <c r="H49" t="s">
         <v>197</v>
       </c>
-      <c r="J49" s="2">
+      <c r="I49" s="2">
         <v>6.7013730000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2726,14 +2728,14 @@
       <c r="G50">
         <v>2.805086673239181E-3</v>
       </c>
-      <c r="I50" t="s">
+      <c r="H50" t="s">
         <v>198</v>
       </c>
-      <c r="J50" s="2">
+      <c r="I50" s="2">
         <v>6.8023160000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2755,14 +2757,14 @@
       <c r="G51">
         <v>2.7285521065512869E-3</v>
       </c>
-      <c r="I51" t="s">
+      <c r="H51" t="s">
         <v>199</v>
       </c>
-      <c r="J51" s="2">
+      <c r="I51" s="2">
         <v>6.9018240000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2784,14 +2786,14 @@
       <c r="G52">
         <v>2.5809592594512021E-3</v>
       </c>
-      <c r="I52" t="s">
+      <c r="H52" t="s">
         <v>200</v>
       </c>
-      <c r="J52" s="2">
+      <c r="I52" s="2">
         <v>7.001773</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2813,14 +2815,14 @@
       <c r="G53">
         <v>2.6463006672250281E-3</v>
       </c>
-      <c r="I53" t="s">
+      <c r="H53" t="s">
         <v>201</v>
       </c>
-      <c r="J53" s="2">
+      <c r="I53" s="2">
         <v>7.1027120000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2842,14 +2844,14 @@
       <c r="G54">
         <v>2.6589534808458318E-3</v>
       </c>
-      <c r="I54" t="s">
+      <c r="H54" t="s">
         <v>202</v>
       </c>
-      <c r="J54" s="2">
+      <c r="I54" s="2">
         <v>7.2016619999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2871,14 +2873,14 @@
       <c r="G55">
         <v>2.6969400027434709E-3</v>
       </c>
-      <c r="I55" t="s">
+      <c r="H55" t="s">
         <v>203</v>
       </c>
-      <c r="J55" s="2">
+      <c r="I55" s="2">
         <v>7.3205900000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2900,14 +2902,14 @@
       <c r="G56">
         <v>2.5388500224419559E-3</v>
       </c>
-      <c r="I56" t="s">
+      <c r="H56" t="s">
         <v>204</v>
       </c>
-      <c r="J56" s="2">
+      <c r="I56" s="2">
         <v>7.4055470000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2929,14 +2931,14 @@
       <c r="G57">
         <v>2.6700085094598981E-3</v>
       </c>
-      <c r="I57" t="s">
+      <c r="H57" t="s">
         <v>205</v>
       </c>
-      <c r="J57" s="2">
+      <c r="I57" s="2">
         <v>7.5020910000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2958,14 +2960,14 @@
       <c r="G58">
         <v>2.7340608436954481E-3</v>
       </c>
-      <c r="I58" t="s">
+      <c r="H58" t="s">
         <v>206</v>
       </c>
-      <c r="J58" s="2">
+      <c r="I58" s="2">
         <v>7.6010359999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2987,14 +2989,14 @@
       <c r="G59">
         <v>2.820017520143491E-3</v>
       </c>
-      <c r="I59" t="s">
+      <c r="H59" t="s">
         <v>207</v>
       </c>
-      <c r="J59" s="2">
+      <c r="I59" s="2">
         <v>7.7019799999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3016,14 +3018,14 @@
       <c r="G60">
         <v>2.8129747522193048E-3</v>
       </c>
-      <c r="I60" t="s">
+      <c r="H60" t="s">
         <v>208</v>
       </c>
-      <c r="J60" s="2">
+      <c r="I60" s="2">
         <v>7.8009219999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3045,14 +3047,14 @@
       <c r="G61">
         <v>2.70664525197811E-3</v>
       </c>
-      <c r="I61" t="s">
+      <c r="H61" t="s">
         <v>209</v>
       </c>
-      <c r="J61" s="2">
+      <c r="I61" s="2">
         <v>7.9008669999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3074,14 +3076,14 @@
       <c r="G62">
         <v>2.7115104343473509E-3</v>
       </c>
-      <c r="I62" t="s">
+      <c r="H62" t="s">
         <v>210</v>
       </c>
-      <c r="J62" s="2">
+      <c r="I62" s="2">
         <v>8.0018119999999993</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3103,14 +3105,14 @@
       <c r="G63">
         <v>2.8590772228842009E-3</v>
       </c>
-      <c r="I63" t="s">
+      <c r="H63" t="s">
         <v>211</v>
       </c>
-      <c r="J63" s="2">
+      <c r="I63" s="2">
         <v>8.1027559999999994</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3132,14 +3134,14 @@
       <c r="G64">
         <v>2.888445191811537E-3</v>
       </c>
-      <c r="I64" t="s">
+      <c r="H64" t="s">
         <v>212</v>
       </c>
-      <c r="J64" s="2">
+      <c r="I64" s="2">
         <v>8.2027020000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3161,14 +3163,14 @@
       <c r="G65">
         <v>2.7414891456152379E-3</v>
       </c>
-      <c r="I65" t="s">
+      <c r="H65" t="s">
         <v>213</v>
       </c>
-      <c r="J65" s="2">
+      <c r="I65" s="2">
         <v>8.3106439999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3190,14 +3192,14 @@
       <c r="G66">
         <v>2.905033261993822E-3</v>
       </c>
-      <c r="I66" t="s">
+      <c r="H66" t="s">
         <v>214</v>
       </c>
-      <c r="J66" s="2">
+      <c r="I66" s="2">
         <v>8.4035879999999992</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3219,14 +3221,14 @@
       <c r="G67">
         <v>2.9161065914318982E-3</v>
       </c>
-      <c r="I67" t="s">
+      <c r="H67" t="s">
         <v>215</v>
       </c>
-      <c r="J67" s="2">
+      <c r="I67" s="2">
         <v>8.5021199999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3248,14 +3250,14 @@
       <c r="G68">
         <v>2.7049241018342099E-3</v>
       </c>
-      <c r="I68" t="s">
+      <c r="H68" t="s">
         <v>216</v>
       </c>
-      <c r="J68" s="2">
+      <c r="I68" s="2">
         <v>8.6040609999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3277,14 +3279,14 @@
       <c r="G69">
         <v>2.8023510999765511E-3</v>
       </c>
-      <c r="I69" t="s">
+      <c r="H69" t="s">
         <v>217</v>
       </c>
-      <c r="J69" s="2">
+      <c r="I69" s="2">
         <v>8.7005459999999992</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3306,14 +3308,14 @@
       <c r="G70">
         <v>2.8985234166872759E-3</v>
       </c>
-      <c r="I70" t="s">
+      <c r="H70" t="s">
         <v>218</v>
       </c>
-      <c r="J70" s="2">
+      <c r="I70" s="2">
         <v>8.802486</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3335,14 +3337,14 @@
       <c r="G71">
         <v>2.9821479589101571E-3</v>
       </c>
-      <c r="I71" t="s">
+      <c r="H71" t="s">
         <v>219</v>
       </c>
-      <c r="J71" s="2">
+      <c r="I71" s="2">
         <v>8.9024350000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3364,14 +3366,14 @@
       <c r="G72">
         <v>2.9371265756177709E-3</v>
       </c>
-      <c r="I72" t="s">
+      <c r="H72" t="s">
         <v>220</v>
       </c>
-      <c r="J72" s="2">
+      <c r="I72" s="2">
         <v>9.0033770000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3393,14 +3395,14 @@
       <c r="G73">
         <v>3.116505219242323E-3</v>
       </c>
-      <c r="I73" t="s">
+      <c r="H73" t="s">
         <v>221</v>
       </c>
-      <c r="J73" s="2">
+      <c r="I73" s="2">
         <v>9.1033229999999996</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3422,14 +3424,14 @@
       <c r="G74">
         <v>3.1416117459036092E-3</v>
       </c>
-      <c r="I74" t="s">
+      <c r="H74" t="s">
         <v>222</v>
       </c>
-      <c r="J74" s="2">
+      <c r="I74" s="2">
         <v>9.2032629999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3451,14 +3453,14 @@
       <c r="G75">
         <v>3.2367076029408181E-3</v>
       </c>
-      <c r="I75" t="s">
+      <c r="H75" t="s">
         <v>223</v>
       </c>
-      <c r="J75" s="2">
+      <c r="I75" s="2">
         <v>9.3062059999999995</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3480,14 +3482,14 @@
       <c r="G76">
         <v>3.320503858725283E-3</v>
       </c>
-      <c r="I76" t="s">
+      <c r="H76" t="s">
         <v>224</v>
       </c>
-      <c r="J76" s="2">
+      <c r="I76" s="2">
         <v>9.4011549999999993</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3509,14 +3511,14 @@
       <c r="G77">
         <v>3.319710013459121E-3</v>
       </c>
-      <c r="I77" t="s">
+      <c r="H77" t="s">
         <v>225</v>
       </c>
-      <c r="J77" s="2">
+      <c r="I77" s="2">
         <v>9.5032650000000007</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3538,14 +3540,14 @@
       <c r="G78">
         <v>3.5290430133553441E-3</v>
       </c>
-      <c r="I78" t="s">
+      <c r="H78" t="s">
         <v>226</v>
       </c>
-      <c r="J78" s="2">
+      <c r="I78" s="2">
         <v>9.6032100000000007</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3567,14 +3569,14 @@
       <c r="G79">
         <v>3.525903313877525E-3</v>
       </c>
-      <c r="I79" t="s">
+      <c r="H79" t="s">
         <v>227</v>
       </c>
-      <c r="J79" s="2">
+      <c r="I79" s="2">
         <v>9.7031539999999996</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3596,14 +3598,14 @@
       <c r="G80">
         <v>3.539699820431179E-3</v>
       </c>
-      <c r="I80" t="s">
+      <c r="H80" t="s">
         <v>228</v>
       </c>
-      <c r="J80" s="2">
+      <c r="I80" s="2">
         <v>9.8030969999999993</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3625,14 +3627,14 @@
       <c r="G81">
         <v>3.5014679665040312E-3</v>
       </c>
-      <c r="I81" t="s">
+      <c r="H81" t="s">
         <v>229</v>
       </c>
-      <c r="J81" s="2">
+      <c r="I81" s="2">
         <v>9.9030430000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3654,14 +3656,14 @@
       <c r="G82">
         <v>3.5754739457641762E-3</v>
       </c>
-      <c r="I82" t="s">
+      <c r="H82" t="s">
         <v>230</v>
       </c>
-      <c r="J82" s="2">
+      <c r="I82" s="2">
         <v>10.00299</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3683,14 +3685,14 @@
       <c r="G83">
         <v>3.690755421157097E-3</v>
       </c>
-      <c r="I83" t="s">
+      <c r="H83" t="s">
         <v>231</v>
       </c>
-      <c r="J83" s="2">
+      <c r="I83" s="2">
         <v>10.10393</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3712,14 +3714,14 @@
       <c r="G84">
         <v>3.6032290780488399E-3</v>
       </c>
-      <c r="I84" t="s">
+      <c r="H84" t="s">
         <v>232</v>
       </c>
-      <c r="J84" s="2">
+      <c r="I84" s="2">
         <v>10.20388</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3741,14 +3743,14 @@
       <c r="G85">
         <v>3.6976998752599501E-3</v>
       </c>
-      <c r="I85" t="s">
+      <c r="H85" t="s">
         <v>233</v>
       </c>
-      <c r="J85" s="2">
+      <c r="I85" s="2">
         <v>10.32381</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3770,14 +3772,14 @@
       <c r="G86">
         <v>3.8230395316828339E-3</v>
       </c>
-      <c r="I86" t="s">
+      <c r="H86" t="s">
         <v>234</v>
       </c>
-      <c r="J86" s="2">
+      <c r="I86" s="2">
         <v>10.41076</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3799,14 +3801,14 @@
       <c r="G87">
         <v>3.5901193362487291E-3</v>
       </c>
-      <c r="I87" t="s">
+      <c r="H87" t="s">
         <v>235</v>
       </c>
-      <c r="J87" s="2">
+      <c r="I87" s="2">
         <v>10.50371</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3828,14 +3830,14 @@
       <c r="G88">
         <v>3.6742819147856788E-3</v>
       </c>
-      <c r="I88" t="s">
+      <c r="H88" t="s">
         <v>236</v>
       </c>
-      <c r="J88" s="2">
+      <c r="I88" s="2">
         <v>10.604200000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3857,14 +3859,14 @@
       <c r="G89">
         <v>3.703546197867258E-3</v>
       </c>
-      <c r="I89" t="s">
+      <c r="H89" t="s">
         <v>237</v>
       </c>
-      <c r="J89" s="2">
+      <c r="I89" s="2">
         <v>10.70323</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3886,14 +3888,14 @@
       <c r="G90">
         <v>3.9883236594157627E-3</v>
       </c>
-      <c r="I90" t="s">
+      <c r="H90" t="s">
         <v>238</v>
       </c>
-      <c r="J90" s="2">
+      <c r="I90" s="2">
         <v>10.80217</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3915,14 +3917,14 @@
       <c r="G91">
         <v>4.0198253585250164E-3</v>
       </c>
-      <c r="I91" t="s">
+      <c r="H91" t="s">
         <v>239</v>
       </c>
-      <c r="J91" s="2">
+      <c r="I91" s="2">
         <v>10.90268</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3944,14 +3946,14 @@
       <c r="G92">
         <v>4.19288966668403E-3</v>
       </c>
-      <c r="I92" t="s">
+      <c r="H92" t="s">
         <v>240</v>
       </c>
-      <c r="J92" s="2">
+      <c r="I92" s="2">
         <v>11.002610000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3973,14 +3975,14 @@
       <c r="G93">
         <v>4.3574946908833323E-3</v>
       </c>
-      <c r="I93" t="s">
+      <c r="H93" t="s">
         <v>241</v>
       </c>
-      <c r="J93" s="2">
+      <c r="I93" s="2">
         <v>11.104559999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4002,14 +4004,14 @@
       <c r="G94">
         <v>4.3548347758252956E-3</v>
       </c>
-      <c r="I94" t="s">
+      <c r="H94" t="s">
         <v>242</v>
       </c>
-      <c r="J94" s="2">
+      <c r="I94" s="2">
         <v>11.202500000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4031,14 +4033,14 @@
       <c r="G95">
         <v>4.3169793997831262E-3</v>
       </c>
-      <c r="I95" t="s">
+      <c r="H95" t="s">
         <v>243</v>
       </c>
-      <c r="J95" s="2">
+      <c r="I95" s="2">
         <v>11.32044</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4060,14 +4062,14 @@
       <c r="G96">
         <v>4.2158400073313753E-3</v>
       </c>
-      <c r="I96" t="s">
+      <c r="H96" t="s">
         <v>244</v>
       </c>
-      <c r="J96" s="2">
+      <c r="I96" s="2">
         <v>11.405390000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4089,14 +4091,14 @@
       <c r="G97">
         <v>4.3203214386622222E-3</v>
       </c>
-      <c r="I97" t="s">
+      <c r="H97" t="s">
         <v>245</v>
       </c>
-      <c r="J97" s="2">
+      <c r="I97" s="2">
         <v>11.50534</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4118,14 +4120,14 @@
       <c r="G98">
         <v>4.4401393823230032E-3</v>
       </c>
-      <c r="I98" t="s">
+      <c r="H98" t="s">
         <v>246</v>
       </c>
-      <c r="J98" s="2">
+      <c r="I98" s="2">
         <v>11.60441</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4147,14 +4149,14 @@
       <c r="G99">
         <v>4.2701033084484958E-3</v>
       </c>
-      <c r="I99" t="s">
+      <c r="H99" t="s">
         <v>247</v>
       </c>
-      <c r="J99" s="2">
+      <c r="I99" s="2">
         <v>11.70435</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4176,14 +4178,14 @@
       <c r="G100">
         <v>4.2753523949713816E-3</v>
       </c>
-      <c r="I100" t="s">
+      <c r="H100" t="s">
         <v>248</v>
       </c>
-      <c r="J100" s="2">
+      <c r="I100" s="2">
         <v>11.805300000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4205,14 +4207,14 @@
       <c r="G101">
         <v>4.5723581165267937E-3</v>
       </c>
-      <c r="I101" t="s">
+      <c r="H101" t="s">
         <v>249</v>
       </c>
-      <c r="J101" s="2">
+      <c r="I101" s="2">
         <v>11.905239999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4234,14 +4236,14 @@
       <c r="G102">
         <v>4.4894997960540717E-3</v>
       </c>
-      <c r="I102" t="s">
+      <c r="H102" t="s">
         <v>250</v>
       </c>
-      <c r="J102" s="2">
+      <c r="I102" s="2">
         <v>12.00319</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4263,14 +4265,14 @@
       <c r="G103">
         <v>4.7107660263456331E-3</v>
       </c>
-      <c r="I103" t="s">
+      <c r="H103" t="s">
         <v>251</v>
       </c>
-      <c r="J103" s="2">
+      <c r="I103" s="2">
         <v>12.10413</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4292,14 +4294,14 @@
       <c r="G104">
         <v>4.8827799019753931E-3</v>
       </c>
-      <c r="I104" t="s">
+      <c r="H104" t="s">
         <v>252</v>
       </c>
-      <c r="J104" s="2">
+      <c r="I104" s="2">
         <v>12.20551</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4321,14 +4323,14 @@
       <c r="G105">
         <v>4.9797381964943304E-3</v>
       </c>
-      <c r="I105" t="s">
+      <c r="H105" t="s">
         <v>253</v>
       </c>
-      <c r="J105" s="2">
+      <c r="I105" s="2">
         <v>12.321440000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4350,14 +4352,14 @@
       <c r="G106">
         <v>5.0662983353658769E-3</v>
       </c>
-      <c r="I106" t="s">
+      <c r="H106" t="s">
         <v>254</v>
       </c>
-      <c r="J106" s="2">
+      <c r="I106" s="2">
         <v>12.407389999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4379,14 +4381,14 @@
       <c r="G107">
         <v>5.192089052398768E-3</v>
       </c>
-      <c r="I107" t="s">
+      <c r="H107" t="s">
         <v>255</v>
       </c>
-      <c r="J107" s="2">
+      <c r="I107" s="2">
         <v>12.50535</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4408,14 +4410,14 @@
       <c r="G108">
         <v>5.3863999937580256E-3</v>
       </c>
-      <c r="I108" t="s">
+      <c r="H108" t="s">
         <v>256</v>
       </c>
-      <c r="J108" s="2">
+      <c r="I108" s="2">
         <v>12.60289</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4437,14 +4439,14 @@
       <c r="G109">
         <v>5.452516762388746E-3</v>
       </c>
-      <c r="I109" t="s">
+      <c r="H109" t="s">
         <v>257</v>
       </c>
-      <c r="J109" s="2">
+      <c r="I109" s="2">
         <v>12.704929999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4466,14 +4468,14 @@
       <c r="G110">
         <v>5.8112205890931837E-3</v>
       </c>
-      <c r="I110" t="s">
+      <c r="H110" t="s">
         <v>258</v>
       </c>
-      <c r="J110" s="2">
+      <c r="I110" s="2">
         <v>12.804880000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -4495,14 +4497,14 @@
       <c r="G111">
         <v>5.7366889409927154E-3</v>
       </c>
-      <c r="I111" t="s">
+      <c r="H111" t="s">
         <v>259</v>
       </c>
-      <c r="J111" s="2">
+      <c r="I111" s="2">
         <v>12.90483</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -4524,14 +4526,14 @@
       <c r="G112">
         <v>5.8951973790638884E-3</v>
       </c>
-      <c r="I112" t="s">
+      <c r="H112" t="s">
         <v>260</v>
       </c>
-      <c r="J112" s="2">
+      <c r="I112" s="2">
         <v>13.003769999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4553,14 +4555,14 @@
       <c r="G113">
         <v>6.0483635239482426E-3</v>
       </c>
-      <c r="I113" t="s">
+      <c r="H113" t="s">
         <v>261</v>
       </c>
-      <c r="J113" s="2">
+      <c r="I113" s="2">
         <v>13.10371</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4582,14 +4584,14 @@
       <c r="G114">
         <v>6.2343879814053364E-3</v>
       </c>
-      <c r="I114" t="s">
+      <c r="H114" t="s">
         <v>262</v>
       </c>
-      <c r="J114" s="2">
+      <c r="I114" s="2">
         <v>13.203659999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4611,14 +4613,14 @@
       <c r="G115">
         <v>6.2211238986587987E-3</v>
       </c>
-      <c r="I115" t="s">
+      <c r="H115" t="s">
         <v>263</v>
       </c>
-      <c r="J115" s="2">
+      <c r="I115" s="2">
         <v>13.31461</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4640,14 +4642,14 @@
       <c r="G116">
         <v>6.3905169154605899E-3</v>
       </c>
-      <c r="I116" t="s">
+      <c r="H116" t="s">
         <v>264</v>
       </c>
-      <c r="J116" s="2">
+      <c r="I116" s="2">
         <v>13.403549999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4669,14 +4671,14 @@
       <c r="G117">
         <v>6.625498628188637E-3</v>
       </c>
-      <c r="I117" t="s">
+      <c r="H117" t="s">
         <v>265</v>
       </c>
-      <c r="J117" s="2">
+      <c r="I117" s="2">
         <v>13.504490000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4698,14 +4700,14 @@
       <c r="G118">
         <v>6.5776452714097237E-3</v>
       </c>
-      <c r="I118" t="s">
+      <c r="H118" t="s">
         <v>266</v>
       </c>
-      <c r="J118" s="2">
+      <c r="I118" s="2">
         <v>13.61199</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4727,14 +4729,14 @@
       <c r="G119">
         <v>6.8051325157477242E-3</v>
       </c>
-      <c r="I119" t="s">
+      <c r="H119" t="s">
         <v>267</v>
       </c>
-      <c r="J119" s="2">
+      <c r="I119" s="2">
         <v>13.70594</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4756,14 +4758,14 @@
       <c r="G120">
         <v>6.7104637910635739E-3</v>
       </c>
-      <c r="I120" t="s">
+      <c r="H120" t="s">
         <v>268</v>
       </c>
-      <c r="J120" s="2">
+      <c r="I120" s="2">
         <v>13.80589</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4785,14 +4787,14 @@
       <c r="G121">
         <v>6.9531027257740711E-3</v>
       </c>
-      <c r="I121" t="s">
+      <c r="H121" t="s">
         <v>269</v>
       </c>
-      <c r="J121" s="2">
+      <c r="I121" s="2">
         <v>13.910819999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4814,14 +4816,14 @@
       <c r="G122">
         <v>6.8148599305806086E-3</v>
       </c>
-      <c r="I122" t="s">
+      <c r="H122" t="s">
         <v>270</v>
       </c>
-      <c r="J122" s="2">
+      <c r="I122" s="2">
         <v>14.00977</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4843,14 +4845,14 @@
       <c r="G123">
         <v>6.8819974784251874E-3</v>
       </c>
-      <c r="I123" t="s">
+      <c r="H123" t="s">
         <v>271</v>
       </c>
-      <c r="J123" s="2">
+      <c r="I123" s="2">
         <v>14.10572</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4872,14 +4874,14 @@
       <c r="G124">
         <v>6.7796096824105636E-3</v>
       </c>
-      <c r="I124" t="s">
+      <c r="H124" t="s">
         <v>272</v>
       </c>
-      <c r="J124" s="2">
+      <c r="I124" s="2">
         <v>14.20567</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4901,14 +4903,14 @@
       <c r="G125">
         <v>6.8152978252363338E-3</v>
       </c>
-      <c r="I125" t="s">
+      <c r="H125" t="s">
         <v>273</v>
       </c>
-      <c r="J125" s="2">
+      <c r="I125" s="2">
         <v>14.30761</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4930,14 +4932,14 @@
       <c r="G126">
         <v>6.7596221810886474E-3</v>
       </c>
-      <c r="I126" t="s">
+      <c r="H126" t="s">
         <v>274</v>
       </c>
-      <c r="J126" s="2">
+      <c r="I126" s="2">
         <v>14.40455</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4959,14 +4961,14 @@
       <c r="G127">
         <v>6.6903704089374396E-3</v>
       </c>
-      <c r="I127" t="s">
+      <c r="H127" t="s">
         <v>275</v>
       </c>
-      <c r="J127" s="2">
+      <c r="I127" s="2">
         <v>14.5055</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4988,14 +4990,14 @@
       <c r="G128">
         <v>6.7359200155963101E-3</v>
       </c>
-      <c r="I128" t="s">
+      <c r="H128" t="s">
         <v>276</v>
       </c>
-      <c r="J128" s="2">
+      <c r="I128" s="2">
         <v>14.604039999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5017,14 +5019,14 @@
       <c r="G129">
         <v>6.568653976395146E-3</v>
       </c>
-      <c r="I129" t="s">
+      <c r="H129" t="s">
         <v>277</v>
       </c>
-      <c r="J129" s="2">
+      <c r="I129" s="2">
         <v>14.70599</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5046,14 +5048,14 @@
       <c r="G130">
         <v>6.5138713163215038E-3</v>
       </c>
-      <c r="I130" t="s">
+      <c r="H130" t="s">
         <v>278</v>
       </c>
-      <c r="J130" s="2">
+      <c r="I130" s="2">
         <v>14.80593</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5075,14 +5077,14 @@
       <c r="G131">
         <v>6.5455237099887788E-3</v>
       </c>
-      <c r="I131" t="s">
+      <c r="H131" t="s">
         <v>279</v>
       </c>
-      <c r="J131" s="2">
+      <c r="I131" s="2">
         <v>14.906890000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5104,14 +5106,14 @@
       <c r="G132">
         <v>6.5494756670118458E-3</v>
       </c>
-      <c r="I132" t="s">
+      <c r="H132" t="s">
         <v>280</v>
       </c>
-      <c r="J132" s="2">
+      <c r="I132" s="2">
         <v>15.006819999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5133,14 +5135,14 @@
       <c r="G133">
         <v>6.6182771273132924E-3</v>
       </c>
-      <c r="I133" t="s">
+      <c r="H133" t="s">
         <v>281</v>
       </c>
-      <c r="J133" s="2">
+      <c r="I133" s="2">
         <v>15.106769999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5162,14 +5164,14 @@
       <c r="G134">
         <v>6.6318410588348479E-3</v>
       </c>
-      <c r="I134" t="s">
+      <c r="H134" t="s">
         <v>282</v>
       </c>
-      <c r="J134" s="2">
+      <c r="I134" s="2">
         <v>15.20673</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5191,14 +5193,14 @@
       <c r="G135">
         <v>6.6537732340751516E-3</v>
       </c>
-      <c r="I135" t="s">
+      <c r="H135" t="s">
         <v>283</v>
       </c>
-      <c r="J135" s="2">
+      <c r="I135" s="2">
         <v>15.30965</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5220,14 +5222,14 @@
       <c r="G136">
         <v>6.7283167386178516E-3</v>
       </c>
-      <c r="I136" t="s">
+      <c r="H136" t="s">
         <v>284</v>
       </c>
-      <c r="J136" s="2">
+      <c r="I136" s="2">
         <v>15.406599999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5249,14 +5251,14 @@
       <c r="G137">
         <v>6.6283759721712581E-3</v>
       </c>
-      <c r="I137" t="s">
+      <c r="H137" t="s">
         <v>285</v>
       </c>
-      <c r="J137" s="2">
+      <c r="I137" s="2">
         <v>15.506539999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5278,14 +5280,14 @@
       <c r="G138">
         <v>6.6335384952210018E-3</v>
       </c>
-      <c r="I138" t="s">
+      <c r="H138" t="s">
         <v>286</v>
       </c>
-      <c r="J138" s="2">
+      <c r="I138" s="2">
         <v>15.60426</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5307,14 +5309,14 @@
       <c r="G139">
         <v>6.708327278448621E-3</v>
       </c>
-      <c r="I139" t="s">
+      <c r="H139" t="s">
         <v>287</v>
       </c>
-      <c r="J139" s="2">
+      <c r="I139" s="2">
         <v>15.708869999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5336,14 +5338,14 @@
       <c r="G140">
         <v>6.6098369375741494E-3</v>
       </c>
-      <c r="I140" t="s">
+      <c r="H140" t="s">
         <v>288</v>
       </c>
-      <c r="J140" s="2">
+      <c r="I140" s="2">
         <v>15.805300000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5365,14 +5367,14 @@
       <c r="G141">
         <v>6.6611075403068976E-3</v>
       </c>
-      <c r="I141" t="s">
+      <c r="H141" t="s">
         <v>289</v>
       </c>
-      <c r="J141" s="2">
+      <c r="I141" s="2">
         <v>15.90673</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5394,14 +5396,14 @@
       <c r="G142">
         <v>6.6022322914015674E-3</v>
       </c>
-      <c r="I142" t="s">
+      <c r="H142" t="s">
         <v>290</v>
       </c>
-      <c r="J142" s="2">
+      <c r="I142" s="2">
         <v>16.006720000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5423,14 +5425,14 @@
       <c r="G143">
         <v>6.7199414883632128E-3</v>
       </c>
-      <c r="I143" t="s">
+      <c r="H143" t="s">
         <v>291</v>
       </c>
-      <c r="J143" s="2">
+      <c r="I143" s="2">
         <v>16.1097</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5452,14 +5454,14 @@
       <c r="G144">
         <v>1.7209665272085829E-2</v>
       </c>
-      <c r="I144" t="s">
+      <c r="H144" t="s">
         <v>292</v>
       </c>
-      <c r="J144" s="2">
+      <c r="I144" s="2">
         <v>16.20523</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5481,39 +5483,39 @@
       <c r="G145">
         <v>0.35784876827899048</v>
       </c>
-      <c r="I145" t="s">
+      <c r="H145" t="s">
         <v>293</v>
       </c>
-      <c r="J145" s="2">
+      <c r="I145" s="2">
         <v>16.322199999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J146" s="2"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J147" s="2"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J148" s="2"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J149" s="2"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J150" s="2"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J151" s="2"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J152" s="2"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J153" s="2"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J154" s="2"/>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I146" s="2"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I147" s="2"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I148" s="2"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I149" s="2"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I150" s="2"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I151" s="2"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I152" s="2"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I153" s="2"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I154" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed full analysis and saving of data in post processing TODO: Move analysis from examples to the package.
</commit_message>
<xml_diff>
--- a/examples/imada_ut/output/myexcel-withTimes.xlsx
+++ b/examples/imada_ut/output/myexcel-withTimes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_sandbox\research\hmu.materialslab.tools\examples\imada_ut\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_sandbox\hmu\hmu.materialslab.tools\examples\imada_ut\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30481D4A-EF8C-4778-80B4-C7AE38B456D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38667475-4837-47C5-B479-156B6F7A3F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="7935" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -970,7 +970,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1277,18 +1277,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145:XFD145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.36328125" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>-9.8860740000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>1.4526502261841669E-4</v>
       </c>
       <c r="F3">
-        <v>-1.15117539585868E-4</v>
+        <v>4.9376186288497333E-5</v>
       </c>
       <c r="G3">
         <v>2.2616582916681731E-4</v>
@@ -1372,7 +1372,7 @@
         <v>-1.0170940000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>3.680200592182631E-4</v>
       </c>
       <c r="F4">
-        <v>-3.1519720067530881E-4</v>
+        <v>-1.3312295453497101E-4</v>
       </c>
       <c r="G4">
         <v>4.7997199699056778E-4</v>
@@ -1401,7 +1401,7 @@
         <v>2.2577229999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>2.720677120707695E-4</v>
       </c>
       <c r="F5">
-        <v>-2.0661024550209481E-4</v>
+        <v>-1.3640146619020691E-4</v>
       </c>
       <c r="G5">
         <v>4.0821737128361469E-4</v>
@@ -1430,7 +1430,7 @@
         <v>2.3126929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>3.4063886409796689E-4</v>
       </c>
       <c r="F6">
-        <v>-5.5321427873729627E-4</v>
+        <v>-3.9251111220429789E-4</v>
       </c>
       <c r="G6">
         <v>6.0332439772039365E-4</v>
@@ -1459,7 +1459,7 @@
         <v>2.4126370000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>6.1265976405767335E-4</v>
       </c>
       <c r="F7">
-        <v>-9.644233246435113E-5</v>
+        <v>-1.1924874496648259E-4</v>
       </c>
       <c r="G7">
         <v>7.4718692637782877E-4</v>
@@ -1488,7 +1488,7 @@
         <v>2.5046919999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>7.3008711384754861E-4</v>
       </c>
       <c r="F8">
-        <v>-5.2213418367380766E-4</v>
+        <v>-4.6797388916390581E-4</v>
       </c>
       <c r="G8">
         <v>8.7151973213200516E-4</v>
@@ -1517,7 +1517,7 @@
         <v>2.6016360000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>5.1200151654763441E-4</v>
       </c>
       <c r="F9">
-        <v>-3.0184011613311641E-4</v>
+        <v>-3.6810720761731782E-4</v>
       </c>
       <c r="G9">
         <v>9.1668731510869555E-4</v>
@@ -1546,7 +1546,7 @@
         <v>2.7141899999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>7.5499012441646517E-4</v>
       </c>
       <c r="F10">
-        <v>-5.6448957001794425E-4</v>
+        <v>-4.8997320705279916E-4</v>
       </c>
       <c r="G10">
         <v>9.6650691293338287E-4</v>
@@ -1575,7 +1575,7 @@
         <v>2.8301270000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>6.0185801515296768E-4</v>
       </c>
       <c r="F11">
-        <v>-6.1724487778750683E-4</v>
+        <v>-5.1919213735789277E-4</v>
       </c>
       <c r="G11">
         <v>1.028546275008682E-3</v>
@@ -1604,7 +1604,7 @@
         <v>2.9380670000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>5.6335761131653484E-4</v>
       </c>
       <c r="F12">
-        <v>-5.0111040639933978E-4</v>
+        <v>-6.0127668255493801E-4</v>
       </c>
       <c r="G12">
         <v>9.4561857293639609E-4</v>
@@ -1633,7 +1633,7 @@
         <v>3.037013</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>8.2125131632141476E-4</v>
       </c>
       <c r="F13">
-        <v>-6.4158107106262671E-4</v>
+        <v>-3.9816599517511887E-4</v>
       </c>
       <c r="G13">
         <v>9.5810543469415784E-4</v>
@@ -1662,7 +1662,7 @@
         <v>3.1439530000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>7.4432763286844637E-4</v>
       </c>
       <c r="F14">
-        <v>-5.7594464493039804E-4</v>
+        <v>-5.0222451712087564E-4</v>
       </c>
       <c r="G14">
         <v>1.1021920696216349E-3</v>
@@ -1691,7 +1691,7 @@
         <v>3.1989299999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>1.0262075906427449E-3</v>
       </c>
       <c r="F15">
-        <v>-5.0169462984567194E-4</v>
+        <v>-3.6036669072796792E-4</v>
       </c>
       <c r="G15">
         <v>1.046465058260069E-3</v>
@@ -1720,7 +1720,7 @@
         <v>3.3068610000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>8.4476951153988563E-4</v>
       </c>
       <c r="F16">
-        <v>-7.6118558683162252E-4</v>
+        <v>-2.416997923115596E-4</v>
       </c>
       <c r="G16">
         <v>1.1823553741109401E-3</v>
@@ -1749,7 +1749,7 @@
         <v>3.402809</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>8.241707906787004E-4</v>
       </c>
       <c r="F17">
-        <v>-6.4510898750219756E-4</v>
+        <v>-2.0596093088842251E-4</v>
       </c>
       <c r="G17">
         <v>1.2174121640850159E-3</v>
@@ -1778,7 +1778,7 @@
         <v>3.5013239999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>1.066299405405555E-3</v>
       </c>
       <c r="F18">
-        <v>-1.0771606896797961E-3</v>
+        <v>-3.971313903129714E-4</v>
       </c>
       <c r="G18">
         <v>1.055824304757609E-3</v>
@@ -1807,7 +1807,7 @@
         <v>3.6152730000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>7.8050565669277353E-4</v>
       </c>
       <c r="F19">
-        <v>-7.8233703190319788E-4</v>
+        <v>-3.5733473658273502E-4</v>
       </c>
       <c r="G19">
         <v>1.348501250184566E-3</v>
@@ -1836,7 +1836,7 @@
         <v>3.7072059999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>8.091448223994306E-4</v>
       </c>
       <c r="F20">
-        <v>-1.2913756830670909E-3</v>
+        <v>-6.1980505763602602E-4</v>
       </c>
       <c r="G20">
         <v>9.9607194828515901E-4</v>
@@ -1865,7 +1865,7 @@
         <v>3.8341370000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>1.0589357417063799E-3</v>
       </c>
       <c r="F21">
-        <v>-1.3484673732752799E-3</v>
+        <v>-5.8601630146259466E-4</v>
       </c>
       <c r="G21">
         <v>1.084463038221447E-3</v>
@@ -1894,7 +1894,7 @@
         <v>3.9280840000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>8.2400257003777436E-4</v>
       </c>
       <c r="F22">
-        <v>-1.234811393057272E-3</v>
+        <v>-8.16978062863464E-4</v>
       </c>
       <c r="G22">
         <v>1.1404877971580201E-3</v>
@@ -1923,7 +1923,7 @@
         <v>4.0160349999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>9.5894852924766235E-4</v>
       </c>
       <c r="F23">
-        <v>-1.770996130795175E-3</v>
+        <v>-8.8309299879761334E-4</v>
       </c>
       <c r="G23">
         <v>1.1122186244201511E-3</v>
@@ -1952,7 +1952,7 @@
         <v>4.1109859999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>1.030603370844134E-3</v>
       </c>
       <c r="F24">
-        <v>-1.4617829422725831E-3</v>
+        <v>-9.1782112870534942E-4</v>
       </c>
       <c r="G24">
         <v>1.231368427888401E-3</v>
@@ -1981,7 +1981,7 @@
         <v>4.2099279999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>6.9398499677130615E-4</v>
       </c>
       <c r="F25">
-        <v>-2.064291967217489E-3</v>
+        <v>-1.427747406887486E-3</v>
       </c>
       <c r="G25">
         <v>1.274822169217843E-3</v>
@@ -2010,7 +2010,7 @@
         <v>4.3138699999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>1.002329786747631E-3</v>
       </c>
       <c r="F26">
-        <v>-1.9554915830825499E-3</v>
+        <v>-1.135033129024835E-3</v>
       </c>
       <c r="G26">
         <v>1.442655535570266E-3</v>
@@ -2039,7 +2039,7 @@
         <v>4.4138149999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>7.8045441927206203E-4</v>
       </c>
       <c r="F27">
-        <v>-1.854821912259475E-3</v>
+        <v>-1.2133219475302069E-3</v>
       </c>
       <c r="G27">
         <v>1.520950659674196E-3</v>
@@ -2068,7 +2068,7 @@
         <v>4.5033450000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>1.0941362055067599E-3</v>
       </c>
       <c r="F28">
-        <v>-2.036819537521837E-3</v>
+        <v>-1.018043519775818E-3</v>
       </c>
       <c r="G28">
         <v>1.491682385874748E-3</v>
@@ -2097,7 +2097,7 @@
         <v>4.6294190000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>1.1802738219522449E-3</v>
       </c>
       <c r="F29">
-        <v>-2.2927472511709329E-3</v>
+        <v>-1.055072345893165E-3</v>
       </c>
       <c r="G29">
         <v>1.2866140935562369E-3</v>
@@ -2126,7 +2126,7 @@
         <v>4.7238759999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>9.8468034748940112E-4</v>
       </c>
       <c r="F30">
-        <v>-2.325706037542894E-3</v>
+        <v>-1.3582517923999291E-3</v>
       </c>
       <c r="G30">
         <v>1.3448478452996191E-3</v>
@@ -2155,7 +2155,7 @@
         <v>4.8058360000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>1.317750611548228E-3</v>
       </c>
       <c r="F31">
-        <v>-2.6245975460234871E-3</v>
+        <v>-1.557348746162833E-3</v>
       </c>
       <c r="G31">
         <v>1.409396867424128E-3</v>
@@ -2184,7 +2184,7 @@
         <v>4.8997789999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>1.1129784594433041E-3</v>
       </c>
       <c r="F32">
-        <v>-2.691112972647073E-3</v>
+        <v>-1.5008253372287841E-3</v>
       </c>
       <c r="G32">
         <v>1.4339817990805901E-3</v>
@@ -2213,7 +2213,7 @@
         <v>4.999727</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>1.137009777543795E-3</v>
       </c>
       <c r="F33">
-        <v>-3.0233178040993151E-3</v>
+        <v>-1.8781080301861969E-3</v>
       </c>
       <c r="G33">
         <v>1.551335941741666E-3</v>
@@ -2242,7 +2242,7 @@
         <v>5.1006689999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>1.511780561595427E-3</v>
       </c>
       <c r="F34">
-        <v>-3.048637543924578E-3</v>
+        <v>-2.170624142423922E-3</v>
       </c>
       <c r="G34">
         <v>1.6151542938856549E-3</v>
@@ -2271,7 +2271,7 @@
         <v>5.200615</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>1.5503548570476281E-3</v>
       </c>
       <c r="F35">
-        <v>-3.4923255269884968E-3</v>
+        <v>-2.0864109540990562E-3</v>
       </c>
       <c r="G35">
         <v>1.7410306829268171E-3</v>
@@ -2300,7 +2300,7 @@
         <v>5.3035579999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1.208471799399173E-3</v>
       </c>
       <c r="F36">
-        <v>-3.3834668288383139E-3</v>
+        <v>-2.2444454304655069E-3</v>
       </c>
       <c r="G36">
         <v>1.6768072891718609E-3</v>
@@ -2329,7 +2329,7 @@
         <v>5.4035019999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>1.183368125893335E-3</v>
       </c>
       <c r="F37">
-        <v>-3.5417563002942279E-3</v>
+        <v>-2.4687735810579102E-3</v>
       </c>
       <c r="G37">
         <v>2.049375563029021E-3</v>
@@ -2358,7 +2358,7 @@
         <v>5.5010110000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>1.4202266700692029E-3</v>
       </c>
       <c r="F38">
-        <v>-3.5239640269759719E-3</v>
+        <v>-2.7397494521856892E-3</v>
       </c>
       <c r="G38">
         <v>2.0452696150272029E-3</v>
@@ -2387,7 +2387,7 @@
         <v>5.6005520000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>1.7001992114186429E-3</v>
       </c>
       <c r="F39">
-        <v>-3.537443725181365E-3</v>
+        <v>-2.5168599701221928E-3</v>
       </c>
       <c r="G39">
         <v>1.968561878366199E-3</v>
@@ -2416,7 +2416,7 @@
         <v>5.7005049999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>1.5121357331581179E-3</v>
       </c>
       <c r="F40">
-        <v>-3.4596649728179281E-3</v>
+        <v>-2.6935540634730479E-3</v>
       </c>
       <c r="G40">
         <v>1.998093685163232E-3</v>
@@ -2445,7 +2445,7 @@
         <v>5.8004490000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>1.331590218691609E-3</v>
       </c>
       <c r="F41">
-        <v>-3.474909727826327E-3</v>
+        <v>-2.7804433021905569E-3</v>
       </c>
       <c r="G41">
         <v>1.935727914272777E-3</v>
@@ -2474,7 +2474,7 @@
         <v>5.9010090000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>1.4352020867432959E-3</v>
       </c>
       <c r="F42">
-        <v>-3.356791365049541E-3</v>
+        <v>-2.6771825528981098E-3</v>
       </c>
       <c r="G42">
         <v>2.0545958122343828E-3</v>
@@ -2503,7 +2503,7 @@
         <v>6.0019559999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>1.5313615906051481E-3</v>
       </c>
       <c r="F43">
-        <v>-3.3466478896990478E-3</v>
+        <v>-2.9126987662499069E-3</v>
       </c>
       <c r="G43">
         <v>2.277713604271453E-3</v>
@@ -2532,7 +2532,7 @@
         <v>6.1009019999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>1.731204210207133E-3</v>
       </c>
       <c r="F44">
-        <v>-3.3712186327642139E-3</v>
+        <v>-3.2191272251246091E-3</v>
       </c>
       <c r="G44">
         <v>2.2814845670358569E-3</v>
@@ -2561,7 +2561,7 @@
         <v>6.2018440000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>1.4356740895380121E-3</v>
       </c>
       <c r="F45">
-        <v>-3.099789050428836E-3</v>
+        <v>-3.3485649307144149E-3</v>
       </c>
       <c r="G45">
         <v>2.4823075431315892E-3</v>
@@ -2590,7 +2590,7 @@
         <v>6.3017859999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>1.3075939368164459E-3</v>
       </c>
       <c r="F46">
-        <v>-3.040537679938179E-3</v>
+        <v>-3.1987101135163868E-3</v>
       </c>
       <c r="G46">
         <v>2.6127224041367809E-3</v>
@@ -2619,7 +2619,7 @@
         <v>6.3997320000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>1.543731077045186E-3</v>
       </c>
       <c r="F47">
-        <v>-2.9905047490365599E-3</v>
+        <v>-3.4725935791488352E-3</v>
       </c>
       <c r="G47">
         <v>2.7924735354853351E-3</v>
@@ -2648,7 +2648,7 @@
         <v>6.5012699999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1.7418612960355829E-3</v>
       </c>
       <c r="F48">
-        <v>-2.873418869884784E-3</v>
+        <v>-3.735895700709084E-3</v>
       </c>
       <c r="G48">
         <v>2.7529126363685921E-3</v>
@@ -2677,7 +2677,7 @@
         <v>6.6012170000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>1.666817575660556E-3</v>
       </c>
       <c r="F49">
-        <v>-2.7177547223626009E-3</v>
+        <v>-3.712243692504905E-3</v>
       </c>
       <c r="G49">
         <v>2.5477906946928691E-3</v>
@@ -2706,7 +2706,7 @@
         <v>6.7013730000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>1.448417677308566E-3</v>
       </c>
       <c r="F50">
-        <v>-2.633274682879075E-3</v>
+        <v>-3.7455947642717328E-3</v>
       </c>
       <c r="G50">
         <v>2.805086673239181E-3</v>
@@ -2735,7 +2735,7 @@
         <v>6.8023160000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>1.4729845036801541E-3</v>
       </c>
       <c r="F51">
-        <v>-2.6794906228305971E-3</v>
+        <v>-3.9556621234859311E-3</v>
       </c>
       <c r="G51">
         <v>2.7285521065512869E-3</v>
@@ -2764,7 +2764,7 @@
         <v>6.9018240000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>1.713452950201966E-3</v>
       </c>
       <c r="F52">
-        <v>-2.5953771505003958E-3</v>
+        <v>-3.631489384296535E-3</v>
       </c>
       <c r="G52">
         <v>2.5809592594512021E-3</v>
@@ -2793,7 +2793,7 @@
         <v>7.001773</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>2.0390045706781871E-3</v>
       </c>
       <c r="F53">
-        <v>-2.5517852413190611E-3</v>
+        <v>-3.5596394591276529E-3</v>
       </c>
       <c r="G53">
         <v>2.6463006672250281E-3</v>
@@ -2822,7 +2822,7 @@
         <v>7.1027120000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>1.772144205457951E-3</v>
       </c>
       <c r="F54">
-        <v>-2.276924135958524E-3</v>
+        <v>-3.797226526303456E-3</v>
       </c>
       <c r="G54">
         <v>2.6589534808458318E-3</v>
@@ -2851,7 +2851,7 @@
         <v>7.2016619999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>1.6868235175833319E-3</v>
       </c>
       <c r="F55">
-        <v>-2.1084700148248409E-3</v>
+        <v>-3.9084306692328541E-3</v>
       </c>
       <c r="G55">
         <v>2.6969400027434709E-3</v>
@@ -2880,7 +2880,7 @@
         <v>7.3205900000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>1.8410044473272931E-3</v>
       </c>
       <c r="F56">
-        <v>-2.2120872180960509E-3</v>
+        <v>-3.659694489903539E-3</v>
       </c>
       <c r="G56">
         <v>2.5388500224419559E-3</v>
@@ -2909,7 +2909,7 @@
         <v>7.4055470000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>2.081792915788948E-3</v>
       </c>
       <c r="F57">
-        <v>-2.0699383144923279E-3</v>
+        <v>-3.8426104412278249E-3</v>
       </c>
       <c r="G57">
         <v>2.6700085094598981E-3</v>
@@ -2938,7 +2938,7 @@
         <v>7.5020910000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>1.8188966999048799E-3</v>
       </c>
       <c r="F58">
-        <v>-1.750592804453181E-3</v>
+        <v>-3.943232328701282E-3</v>
       </c>
       <c r="G58">
         <v>2.7340608436954481E-3</v>
@@ -2967,7 +2967,7 @@
         <v>7.6010359999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>1.687341647984008E-3</v>
       </c>
       <c r="F59">
-        <v>-1.6306491699213911E-3</v>
+        <v>-3.8663544011772939E-3</v>
       </c>
       <c r="G59">
         <v>2.820017520143491E-3</v>
@@ -2996,7 +2996,7 @@
         <v>7.7019799999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>1.952980001912903E-3</v>
       </c>
       <c r="F60">
-        <v>-1.591141831973124E-3</v>
+        <v>-3.828413460234356E-3</v>
       </c>
       <c r="G60">
         <v>2.8129747522193048E-3</v>
@@ -3025,7 +3025,7 @@
         <v>7.8009219999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>2.269019722181713E-3</v>
       </c>
       <c r="F61">
-        <v>-1.621617407561332E-3</v>
+        <v>-4.0154131050077792E-3</v>
       </c>
       <c r="G61">
         <v>2.70664525197811E-3</v>
@@ -3054,7 +3054,7 @@
         <v>7.9008669999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>1.9711753754647989E-3</v>
       </c>
       <c r="F62">
-        <v>-1.2853784562806641E-3</v>
+        <v>-4.0756910800620284E-3</v>
       </c>
       <c r="G62">
         <v>2.7115104343473509E-3</v>
@@ -3083,7 +3083,7 @@
         <v>8.0018119999999993</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>1.882316578161523E-3</v>
       </c>
       <c r="F63">
-        <v>-1.092372257513585E-3</v>
+        <v>-4.0353725584459984E-3</v>
       </c>
       <c r="G63">
         <v>2.8590772228842009E-3</v>
@@ -3112,7 +3112,7 @@
         <v>8.1027559999999994</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>2.0939829854264261E-3</v>
       </c>
       <c r="F64">
-        <v>-1.1342917924780751E-3</v>
+        <v>-3.9643793936776977E-3</v>
       </c>
       <c r="G64">
         <v>2.888445191811537E-3</v>
@@ -3141,7 +3141,7 @@
         <v>8.2027020000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>2.389543623839903E-3</v>
       </c>
       <c r="F65">
-        <v>-1.104497245140758E-3</v>
+        <v>-4.2544269530134966E-3</v>
       </c>
       <c r="G65">
         <v>2.7414891456152379E-3</v>
@@ -3170,7 +3170,7 @@
         <v>8.3106439999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>2.1867462785184651E-3</v>
       </c>
       <c r="F66">
-        <v>-8.5427388495406111E-4</v>
+        <v>-4.2348835589272786E-3</v>
       </c>
       <c r="G66">
         <v>2.905033261993822E-3</v>
@@ -3199,7 +3199,7 @@
         <v>8.4035879999999992</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>1.9176106619751281E-3</v>
       </c>
       <c r="F67">
-        <v>-5.1153569100234684E-4</v>
+        <v>-4.3046443420687664E-3</v>
       </c>
       <c r="G67">
         <v>2.9161065914318982E-3</v>
@@ -3228,7 +3228,7 @@
         <v>8.5021199999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>2.2360785236066631E-3</v>
       </c>
       <c r="F68">
-        <v>-5.3842054923726478E-4</v>
+        <v>-4.4821764287482826E-3</v>
       </c>
       <c r="G68">
         <v>2.7049241018342099E-3</v>
@@ -3257,7 +3257,7 @@
         <v>8.6040609999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>2.6097890302492358E-3</v>
       </c>
       <c r="F69">
-        <v>-4.7224094405929511E-4</v>
+        <v>-4.5876803446639131E-3</v>
       </c>
       <c r="G69">
         <v>2.8023510999765511E-3</v>
@@ -3286,7 +3286,7 @@
         <v>8.7005459999999992</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>2.4940089907700492E-3</v>
       </c>
       <c r="F70">
-        <v>-1.249293554796725E-4</v>
+        <v>-4.5260843299548548E-3</v>
       </c>
       <c r="G70">
         <v>2.8985234166872759E-3</v>
@@ -3315,7 +3315,7 @@
         <v>8.802486</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>1.936064547978281E-3</v>
       </c>
       <c r="F71">
-        <v>1.209519307988857E-4</v>
+        <v>-4.7535547823046647E-3</v>
       </c>
       <c r="G71">
         <v>2.9821479589101571E-3</v>
@@ -3344,7 +3344,7 @@
         <v>8.9024350000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>2.1532972422416701E-3</v>
       </c>
       <c r="F72">
-        <v>1.8261620736913329E-4</v>
+        <v>-4.9369405248812833E-3</v>
       </c>
       <c r="G72">
         <v>2.9371265756177709E-3</v>
@@ -3373,7 +3373,7 @@
         <v>9.0033770000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>2.5126579793115248E-3</v>
       </c>
       <c r="F73">
-        <v>1.993370293378947E-4</v>
+        <v>-4.9099286540766939E-3</v>
       </c>
       <c r="G73">
         <v>3.116505219242323E-3</v>
@@ -3402,7 +3402,7 @@
         <v>9.1033229999999996</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>2.4799706842262869E-3</v>
       </c>
       <c r="F74">
-        <v>6.1528169377369774E-4</v>
+        <v>-5.4169205210735146E-3</v>
       </c>
       <c r="G74">
         <v>3.1416117459036092E-3</v>
@@ -3431,7 +3431,7 @@
         <v>9.2032629999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>2.3954033679106559E-3</v>
       </c>
       <c r="F75">
-        <v>8.1815979290047276E-4</v>
+        <v>-5.3085900823738657E-3</v>
       </c>
       <c r="G75">
         <v>3.2367076029408181E-3</v>
@@ -3460,7 +3460,7 @@
         <v>9.3062059999999995</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>2.242007312947142E-3</v>
       </c>
       <c r="F76">
-        <v>9.026130220516896E-4</v>
+        <v>-5.4950141122678637E-3</v>
       </c>
       <c r="G76">
         <v>3.320503858725283E-3</v>
@@ -3489,7 +3489,7 @@
         <v>9.4011549999999993</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>2.4904489738980479E-3</v>
       </c>
       <c r="F77">
-        <v>9.8475977984890635E-4</v>
+        <v>-5.4405744761562092E-3</v>
       </c>
       <c r="G77">
         <v>3.319710013459121E-3</v>
@@ -3518,7 +3518,7 @@
         <v>9.5032650000000007</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>2.5472378136520831E-3</v>
       </c>
       <c r="F78">
-        <v>1.4411168717074711E-3</v>
+        <v>-5.7862066226303122E-3</v>
       </c>
       <c r="G78">
         <v>3.5290430133553441E-3</v>
@@ -3547,7 +3547,7 @@
         <v>9.6032100000000007</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>2.497113940048572E-3</v>
       </c>
       <c r="F79">
-        <v>1.761602552770447E-3</v>
+        <v>-5.8764520051100529E-3</v>
       </c>
       <c r="G79">
         <v>3.525903313877525E-3</v>
@@ -3576,7 +3576,7 @@
         <v>9.7031539999999996</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>2.5149742573831761E-3</v>
       </c>
       <c r="F80">
-        <v>1.722761698339542E-3</v>
+        <v>-5.8460734074227789E-3</v>
       </c>
       <c r="G80">
         <v>3.539699820431179E-3</v>
@@ -3605,7 +3605,7 @@
         <v>9.8030969999999993</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>2.3559699534420209E-3</v>
       </c>
       <c r="F81">
-        <v>1.882991103484058E-3</v>
+        <v>-5.6623840277764126E-3</v>
       </c>
       <c r="G81">
         <v>3.5014679665040312E-3</v>
@@ -3634,7 +3634,7 @@
         <v>9.9030430000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>2.4429976696147852E-3</v>
       </c>
       <c r="F82">
-        <v>2.2244313225610402E-3</v>
+        <v>-5.8310328905150184E-3</v>
       </c>
       <c r="G82">
         <v>3.5754739457641762E-3</v>
@@ -3663,7 +3663,7 @@
         <v>10.00299</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>2.4053220689312432E-3</v>
       </c>
       <c r="F83">
-        <v>2.5451191485943762E-3</v>
+        <v>-5.6884078792966654E-3</v>
       </c>
       <c r="G83">
         <v>3.690755421157097E-3</v>
@@ -3692,7 +3692,7 @@
         <v>10.10393</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>2.722105556536627E-3</v>
       </c>
       <c r="F84">
-        <v>2.614264194572316E-3</v>
+        <v>-5.8043113100679656E-3</v>
       </c>
       <c r="G84">
         <v>3.6032290780488399E-3</v>
@@ -3721,7 +3721,7 @@
         <v>10.20388</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>2.7787917563179181E-3</v>
       </c>
       <c r="F85">
-        <v>2.8919791310166661E-3</v>
+        <v>-5.9615545090284201E-3</v>
       </c>
       <c r="G85">
         <v>3.6976998752599501E-3</v>
@@ -3750,7 +3750,7 @@
         <v>10.32381</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>2.502543857772912E-3</v>
       </c>
       <c r="F86">
-        <v>3.0655646876463689E-3</v>
+        <v>-5.9158933823444176E-3</v>
       </c>
       <c r="G86">
         <v>3.8230395316828339E-3</v>
@@ -3779,7 +3779,7 @@
         <v>10.41076</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>2.4020475978238981E-3</v>
       </c>
       <c r="F87">
-        <v>3.3047124210410402E-3</v>
+        <v>-6.0189493904908931E-3</v>
       </c>
       <c r="G87">
         <v>3.5901193362487291E-3</v>
@@ -3808,7 +3808,7 @@
         <v>10.50371</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>2.6292065831154889E-3</v>
       </c>
       <c r="F88">
-        <v>3.6150764410128621E-3</v>
+        <v>-6.2776314304807722E-3</v>
       </c>
       <c r="G88">
         <v>3.6742819147856788E-3</v>
@@ -3837,7 +3837,7 @@
         <v>10.604200000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>2.743591841442938E-3</v>
       </c>
       <c r="F89">
-        <v>3.7898638887724351E-3</v>
+        <v>-6.2380150380242109E-3</v>
       </c>
       <c r="G89">
         <v>3.703546197867258E-3</v>
@@ -3866,7 +3866,7 @@
         <v>10.70323</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>2.8514686428802931E-3</v>
       </c>
       <c r="F90">
-        <v>4.3646912908987534E-3</v>
+        <v>-6.3984844919558704E-3</v>
       </c>
       <c r="G90">
         <v>3.9883236594157627E-3</v>
@@ -3895,7 +3895,7 @@
         <v>10.80217</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>2.491349149974246E-3</v>
       </c>
       <c r="F91">
-        <v>4.6488180377313674E-3</v>
+        <v>-6.5594495810508569E-3</v>
       </c>
       <c r="G91">
         <v>4.0198253585250164E-3</v>
@@ -3924,7 +3924,7 @@
         <v>10.90268</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>2.6030571775925659E-3</v>
       </c>
       <c r="F92">
-        <v>4.6583923977176816E-3</v>
+        <v>-6.8861317537890956E-3</v>
       </c>
       <c r="G92">
         <v>4.19288966668403E-3</v>
@@ -3953,7 +3953,7 @@
         <v>11.002610000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>2.7694262959897481E-3</v>
       </c>
       <c r="F93">
-        <v>4.8566248082973747E-3</v>
+        <v>-6.9339551978850316E-3</v>
       </c>
       <c r="G93">
         <v>4.3574946908833323E-3</v>
@@ -3982,7 +3982,7 @@
         <v>11.104559999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>2.7970114081392371E-3</v>
       </c>
       <c r="F94">
-        <v>5.1401943975938058E-3</v>
+        <v>-6.9619896472557924E-3</v>
       </c>
       <c r="G94">
         <v>4.3548347758252956E-3</v>
@@ -4011,7 +4011,7 @@
         <v>11.202500000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>2.78166776689345E-3</v>
       </c>
       <c r="F95">
-        <v>5.6602504890640804E-3</v>
+        <v>-7.1536551661400922E-3</v>
       </c>
       <c r="G95">
         <v>4.3169793997831262E-3</v>
@@ -4040,7 +4040,7 @@
         <v>11.32044</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>2.8286112301561012E-3</v>
       </c>
       <c r="F96">
-        <v>6.0220265083653973E-3</v>
+        <v>-7.0555148663786994E-3</v>
       </c>
       <c r="G96">
         <v>4.2158400073313753E-3</v>
@@ -4069,7 +4069,7 @@
         <v>11.405390000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>2.7010176597115302E-3</v>
       </c>
       <c r="F97">
-        <v>6.0152668446243002E-3</v>
+        <v>-7.2248480962055078E-3</v>
       </c>
       <c r="G97">
         <v>4.3203214386622222E-3</v>
@@ -4098,7 +4098,7 @@
         <v>11.50534</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>2.7877527149070798E-3</v>
       </c>
       <c r="F98">
-        <v>6.1633736733493986E-3</v>
+        <v>-7.5665610712708749E-3</v>
       </c>
       <c r="G98">
         <v>4.4401393823230032E-3</v>
@@ -4127,7 +4127,7 @@
         <v>11.60441</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>2.7369597623287212E-3</v>
       </c>
       <c r="F99">
-        <v>6.6339554176740147E-3</v>
+        <v>-7.3728533165686632E-3</v>
       </c>
       <c r="G99">
         <v>4.2701033084484958E-3</v>
@@ -4156,7 +4156,7 @@
         <v>11.70435</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>2.9670010571066449E-3</v>
       </c>
       <c r="F100">
-        <v>7.1159609608163494E-3</v>
+        <v>-7.4605321637881156E-3</v>
       </c>
       <c r="G100">
         <v>4.2753523949713816E-3</v>
@@ -4185,7 +4185,7 @@
         <v>11.805300000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>2.935399853972182E-3</v>
       </c>
       <c r="F101">
-        <v>7.6029824592139736E-3</v>
+        <v>-7.6211150607114354E-3</v>
       </c>
       <c r="G101">
         <v>4.5723581165267937E-3</v>
@@ -4214,7 +4214,7 @@
         <v>11.905239999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>2.6150589242436122E-3</v>
       </c>
       <c r="F102">
-        <v>7.9399657586284814E-3</v>
+        <v>-7.9171849336790757E-3</v>
       </c>
       <c r="G102">
         <v>4.4894997960540717E-3</v>
@@ -4243,7 +4243,7 @@
         <v>12.00319</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>2.509516269578928E-3</v>
       </c>
       <c r="F103">
-        <v>8.0157004175652156E-3</v>
+        <v>-8.2398122362610082E-3</v>
       </c>
       <c r="G103">
         <v>4.7107660263456331E-3</v>
@@ -4272,7 +4272,7 @@
         <v>12.10413</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>2.6886828049383958E-3</v>
       </c>
       <c r="F104">
-        <v>8.1801146607950476E-3</v>
+        <v>-8.3376996668126195E-3</v>
       </c>
       <c r="G104">
         <v>4.8827799019753931E-3</v>
@@ -4301,7 +4301,7 @@
         <v>12.20551</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>2.8384440524526111E-3</v>
       </c>
       <c r="F105">
-        <v>8.6624328038149134E-3</v>
+        <v>-8.5422706155281799E-3</v>
       </c>
       <c r="G105">
         <v>4.9797381964943304E-3</v>
@@ -4330,7 +4330,7 @@
         <v>12.321440000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>2.4050598082482168E-3</v>
       </c>
       <c r="F106">
-        <v>9.3433968351600751E-3</v>
+        <v>-8.653787818065797E-3</v>
       </c>
       <c r="G106">
         <v>5.0662983353658769E-3</v>
@@ -4359,7 +4359,7 @@
         <v>12.407389999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>2.452063761241738E-3</v>
       </c>
       <c r="F107">
-        <v>9.7387571064525003E-3</v>
+        <v>-8.8689022907188116E-3</v>
       </c>
       <c r="G107">
         <v>5.192089052398768E-3</v>
@@ -4388,7 +4388,7 @@
         <v>12.50535</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>2.4409376480523958E-3</v>
       </c>
       <c r="F108">
-        <v>9.9516312419017372E-3</v>
+        <v>-9.0529672024572128E-3</v>
       </c>
       <c r="G108">
         <v>5.3863999937580256E-3</v>
@@ -4417,7 +4417,7 @@
         <v>12.60289</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>2.0859580178088761E-3</v>
       </c>
       <c r="F109">
-        <v>1.0242958774630851E-2</v>
+        <v>-9.2976382995087811E-3</v>
       </c>
       <c r="G109">
         <v>5.452516762388746E-3</v>
@@ -4446,7 +4446,7 @@
         <v>12.704929999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>1.906073788059565E-3</v>
       </c>
       <c r="F110">
-        <v>1.082141568231383E-2</v>
+        <v>-9.8550223335617838E-3</v>
       </c>
       <c r="G110">
         <v>5.8112205890931837E-3</v>
@@ -4475,7 +4475,7 @@
         <v>12.804880000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>2.004525508664774E-3</v>
       </c>
       <c r="F111">
-        <v>1.1398251191294969E-2</v>
+        <v>-1.0009577989611881E-2</v>
       </c>
       <c r="G111">
         <v>5.7366889409927154E-3</v>
@@ -4504,7 +4504,7 @@
         <v>12.90483</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>2.0080921082127209E-3</v>
       </c>
       <c r="F112">
-        <v>1.197071018999621E-2</v>
+        <v>-1.0290835108212239E-2</v>
       </c>
       <c r="G112">
         <v>5.8951973790638884E-3</v>
@@ -4533,7 +4533,7 @@
         <v>13.003769999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>1.5656484043918911E-3</v>
       </c>
       <c r="F113">
-        <v>1.2584058059617379E-2</v>
+        <v>-1.036644259601842E-2</v>
       </c>
       <c r="G113">
         <v>6.0483635239482426E-3</v>
@@ -4562,7 +4562,7 @@
         <v>13.10371</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>1.871802529122806E-3</v>
       </c>
       <c r="F114">
-        <v>1.314622027608104E-2</v>
+        <v>-1.0658057965096829E-2</v>
       </c>
       <c r="G114">
         <v>6.2343879814053364E-3</v>
@@ -4591,7 +4591,7 @@
         <v>13.203659999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>2.3360280784096689E-3</v>
       </c>
       <c r="F115">
-        <v>1.352890422341845E-2</v>
+        <v>-1.050518137980958E-2</v>
       </c>
       <c r="G115">
         <v>6.2211238986587987E-3</v>
@@ -4620,7 +4620,7 @@
         <v>13.31461</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>2.6982202948074171E-3</v>
       </c>
       <c r="F116">
-        <v>1.410700292817621E-2</v>
+        <v>-1.0851215715229781E-2</v>
       </c>
       <c r="G116">
         <v>6.3905169154605899E-3</v>
@@ -4649,7 +4649,7 @@
         <v>13.403549999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>2.9240954963338471E-3</v>
       </c>
       <c r="F117">
-        <v>1.496461208086516E-2</v>
+        <v>-1.113326478421436E-2</v>
       </c>
       <c r="G117">
         <v>6.625498628188637E-3</v>
@@ -4678,7 +4678,7 @@
         <v>13.504490000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>3.3507310576760809E-3</v>
       </c>
       <c r="F118">
-        <v>1.5758114645388729E-2</v>
+        <v>-1.1032457433678059E-2</v>
       </c>
       <c r="G118">
         <v>6.5776452714097237E-3</v>
@@ -4707,7 +4707,7 @@
         <v>13.61199</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>3.659122214921835E-3</v>
       </c>
       <c r="F119">
-        <v>1.6383781854028341E-2</v>
+        <v>-1.099651119176575E-2</v>
       </c>
       <c r="G119">
         <v>6.8051325157477242E-3</v>
@@ -4736,7 +4736,7 @@
         <v>13.70594</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>4.1947402317424184E-3</v>
       </c>
       <c r="F120">
-        <v>1.7468460137338899E-2</v>
+        <v>-1.126854222297613E-2</v>
       </c>
       <c r="G120">
         <v>6.7104637910635739E-3</v>
@@ -4765,7 +4765,7 @@
         <v>13.80589</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>4.7508928443529127E-3</v>
       </c>
       <c r="F121">
-        <v>1.8145978948282709E-2</v>
+        <v>-1.148051482236611E-2</v>
       </c>
       <c r="G121">
         <v>6.9531027257740711E-3</v>
@@ -4794,7 +4794,7 @@
         <v>13.910819999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>5.2354263755240108E-3</v>
       </c>
       <c r="F122">
-        <v>1.893338581935141E-2</v>
+        <v>-1.0746912769894869E-2</v>
       </c>
       <c r="G122">
         <v>6.8148599305806086E-3</v>
@@ -4823,7 +4823,7 @@
         <v>14.00977</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>5.917157091147456E-3</v>
       </c>
       <c r="F123">
-        <v>2.0020063120941879E-2</v>
+        <v>-1.1007114518673731E-2</v>
       </c>
       <c r="G123">
         <v>6.8819974784251874E-3</v>
@@ -4852,7 +4852,7 @@
         <v>14.10572</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>5.9239442683518091E-3</v>
       </c>
       <c r="F124">
-        <v>2.0958892543765231E-2</v>
+        <v>-1.083866226285332E-2</v>
       </c>
       <c r="G124">
         <v>6.7796096824105636E-3</v>
@@ -4881,7 +4881,7 @@
         <v>14.20567</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>6.396296412130127E-3</v>
       </c>
       <c r="F125">
-        <v>2.2083521376213819E-2</v>
+        <v>-1.07300482620183E-2</v>
       </c>
       <c r="G125">
         <v>6.8152978252363338E-3</v>
@@ -4910,7 +4910,7 @@
         <v>14.30761</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>6.8098096310236743E-3</v>
       </c>
       <c r="F126">
-        <v>2.3268104150180241E-2</v>
+        <v>-1.054812216461324E-2</v>
       </c>
       <c r="G126">
         <v>6.7596221810886474E-3</v>
@@ -4939,7 +4939,7 @@
         <v>14.40455</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>7.0273862076314364E-3</v>
       </c>
       <c r="F127">
-        <v>2.4206213134491429E-2</v>
+        <v>-1.0767008310739829E-2</v>
       </c>
       <c r="G127">
         <v>6.6903704089374396E-3</v>
@@ -4968,7 +4968,7 @@
         <v>14.5055</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>7.6404375861440178E-3</v>
       </c>
       <c r="F128">
-        <v>2.5546954784387149E-2</v>
+        <v>-1.048850250262991E-2</v>
       </c>
       <c r="G128">
         <v>6.7359200155963101E-3</v>
@@ -4997,7 +4997,7 @@
         <v>14.604039999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>7.8150302468899865E-3</v>
       </c>
       <c r="F129">
-        <v>2.6624724034832011E-2</v>
+        <v>-1.0652557810404049E-2</v>
       </c>
       <c r="G129">
         <v>6.568653976395146E-3</v>
@@ -5026,7 +5026,7 @@
         <v>14.70599</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>7.9964819491054502E-3</v>
       </c>
       <c r="F130">
-        <v>2.7866116985896479E-2</v>
+        <v>-1.074575001178155E-2</v>
       </c>
       <c r="G130">
         <v>6.5138713163215038E-3</v>
@@ -5055,7 +5055,7 @@
         <v>14.80593</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>8.3191563702237417E-3</v>
       </c>
       <c r="F131">
-        <v>2.9138380158022989E-2</v>
+        <v>-1.069553524795647E-2</v>
       </c>
       <c r="G131">
         <v>6.5455237099887788E-3</v>
@@ -5084,7 +5084,7 @@
         <v>14.906890000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>8.4406564474908737E-3</v>
       </c>
       <c r="F132">
-        <v>3.0299059190095571E-2</v>
+        <v>-1.04816982959926E-2</v>
       </c>
       <c r="G132">
         <v>6.5494756670118458E-3</v>
@@ -5113,7 +5113,7 @@
         <v>15.006819999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>8.8464278076525217E-3</v>
       </c>
       <c r="F133">
-        <v>3.1600756907544499E-2</v>
+        <v>-1.0741580016611961E-2</v>
       </c>
       <c r="G133">
         <v>6.6182771273132924E-3</v>
@@ -5142,7 +5142,7 @@
         <v>15.106769999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>9.1217960830023599E-3</v>
       </c>
       <c r="F134">
-        <v>3.2821184004853399E-2</v>
+        <v>-1.0689086137383079E-2</v>
       </c>
       <c r="G134">
         <v>6.6318410588348479E-3</v>
@@ -5171,7 +5171,7 @@
         <v>15.20673</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>9.6317069781132591E-3</v>
       </c>
       <c r="F135">
-        <v>3.404620091718269E-2</v>
+        <v>-1.0748132908729949E-2</v>
       </c>
       <c r="G135">
         <v>6.6537732340751516E-3</v>
@@ -5200,7 +5200,7 @@
         <v>15.30965</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>9.9930257193386988E-3</v>
       </c>
       <c r="F136">
-        <v>3.5415715574060883E-2</v>
+        <v>-1.087506651659494E-2</v>
       </c>
       <c r="G136">
         <v>6.7283167386178516E-3</v>
@@ -5229,7 +5229,7 @@
         <v>15.406599999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>1.0536889084709979E-2</v>
       </c>
       <c r="F137">
-        <v>3.6640382251131892E-2</v>
+        <v>-1.0551549797515819E-2</v>
       </c>
       <c r="G137">
         <v>6.6283759721712581E-3</v>
@@ -5258,7 +5258,7 @@
         <v>15.506539999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>1.117702681472383E-2</v>
       </c>
       <c r="F138">
-        <v>3.7967898268594237E-2</v>
+        <v>-1.0479532010825091E-2</v>
       </c>
       <c r="G138">
         <v>6.6335384952210018E-3</v>
@@ -5287,7 +5287,7 @@
         <v>15.60426</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>1.170054045908726E-2</v>
       </c>
       <c r="F139">
-        <v>3.9304686074531428E-2</v>
+        <v>-1.079006444893439E-2</v>
       </c>
       <c r="G139">
         <v>6.708327278448621E-3</v>
@@ -5316,7 +5316,7 @@
         <v>15.708869999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>1.245896442882541E-2</v>
       </c>
       <c r="F140">
-        <v>4.0574283835114189E-2</v>
+        <v>-1.0320061943936171E-2</v>
       </c>
       <c r="G140">
         <v>6.6098369375741494E-3</v>
@@ -5345,7 +5345,7 @@
         <v>15.805300000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>1.3722742067214209E-2</v>
       </c>
       <c r="F141">
-        <v>4.1845002445862797E-2</v>
+        <v>-1.0167585826826329E-2</v>
       </c>
       <c r="G141">
         <v>6.6611075403068976E-3</v>
@@ -5374,7 +5374,7 @@
         <v>15.90673</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>1.504341309557585E-2</v>
       </c>
       <c r="F142">
-        <v>4.3250146136247669E-2</v>
+        <v>-1.0218403694868761E-2</v>
       </c>
       <c r="G142">
         <v>6.6022322914015674E-3</v>
@@ -5403,7 +5403,7 @@
         <v>16.006720000000001</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>1.8949406479050138E-2</v>
       </c>
       <c r="F143">
-        <v>4.5264494040634387E-2</v>
+        <v>-1.01284308955436E-2</v>
       </c>
       <c r="G143">
         <v>6.7199414883632128E-3</v>
@@ -5432,7 +5432,7 @@
         <v>16.1097</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>2.7156398088909541E-2</v>
       </c>
       <c r="F144">
-        <v>4.9896588866984948E-2</v>
+        <v>-2.3747777806335409E-2</v>
       </c>
       <c r="G144">
         <v>1.7209665272085829E-2</v>
@@ -5461,7 +5461,7 @@
         <v>16.20523</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>0.19560405187064489</v>
       </c>
       <c r="F145">
-        <v>0.15579026361114701</v>
+        <v>-1.5809445514124911E-2</v>
       </c>
       <c r="G145">
         <v>0.35784876827899048</v>
@@ -5490,31 +5490,31 @@
         <v>16.322199999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I146" s="2"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I147" s="2"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I148" s="2"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I149" s="2"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I150" s="2"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I151" s="2"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I152" s="2"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I153" s="2"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I154" s="2"/>
     </row>
   </sheetData>

</xml_diff>